<commit_message>
Incluindo a massa de dados pelo excel
</commit_message>
<xml_diff>
--- a/dadosCadastro.xlsx
+++ b/dadosCadastro.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angra.souza\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angra.souza\Documents\projetoTDD-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D7A624-10A9-428B-A10B-010D326C806F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA3C1C-937B-4B32-A966-DDB5FE7DB3B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69912B33-A1B3-4224-930E-465C0AC4F184}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Nome usuario</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>Confirmar senha</t>
+  </si>
+  <si>
+    <t>(11)970510060</t>
+  </si>
+  <si>
+    <t>(11)970510070</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Brazil</t>
   </si>
 </sst>
 </file>
@@ -480,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA410A54-4D50-40E3-985F-718BE11AC5C5}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,13 +507,14 @@
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,19 +537,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -555,23 +571,26 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
-        <v>11970510060</v>
+      <c r="G2" t="s">
+        <v>26</v>
       </c>
       <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -590,19 +609,22 @@
       <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="G3">
-        <v>11970510070</v>
+      <c r="G3" t="s">
+        <v>27</v>
       </c>
       <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reports e erro na tela de cadastro
</commit_message>
<xml_diff>
--- a/dadosCadastro.xlsx
+++ b/dadosCadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angra.souza\Documents\projetoTDD-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA3C1C-937B-4B32-A966-DDB5FE7DB3B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B235433-CFBA-429B-A6FA-B0401CAA2C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69912B33-A1B3-4224-930E-465C0AC4F184}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Codigo Postal</t>
   </si>
   <si>
-    <t>AngraSouza</t>
-  </si>
-  <si>
     <t>angra.santos@hotmail.com.br</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Brazil</t>
+  </si>
+  <si>
+    <t>AngraSouzaaa</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -554,78 +554,78 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>